<commit_message>
Actualización automática de dinoe.xlsx desde Google Drive
</commit_message>
<xml_diff>
--- a/dinoe.xlsx
+++ b/dinoe.xlsx
@@ -687,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -720,6 +720,9 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="12" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3351,8 +3354,8 @@
       <c r="D6" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="13">
-        <v>57.8</v>
+      <c r="E6" s="14">
+        <v>57.0</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
@@ -3362,7 +3365,7 @@
       <c r="B7" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="15" t="s">
         <v>60</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -3379,7 +3382,7 @@
       <c r="B8" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="15" t="s">
         <v>61</v>
       </c>
       <c r="D8" s="12" t="s">
@@ -3396,7 +3399,7 @@
       <c r="B9" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="15" t="s">
         <v>62</v>
       </c>
       <c r="D9" s="12" t="s">
@@ -3413,7 +3416,7 @@
       <c r="B10" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="15" t="s">
         <v>63</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -3653,13 +3656,13 @@
       <c r="A25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E25" s="13">
@@ -3670,13 +3673,13 @@
       <c r="A26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E26" s="13">
@@ -3687,13 +3690,13 @@
       <c r="A27" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="16" t="s">
         <v>55</v>
       </c>
       <c r="E27" s="13">
@@ -3704,13 +3707,13 @@
       <c r="A28" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="16" t="s">
         <v>55</v>
       </c>
       <c r="E28" s="13"/>
@@ -3719,13 +3722,13 @@
       <c r="A29" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="16" t="s">
         <v>87</v>
       </c>
       <c r="E29" s="13">
@@ -3736,13 +3739,13 @@
       <c r="A30" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="16" t="s">
         <v>90</v>
       </c>
       <c r="E30" s="13">
@@ -3753,13 +3756,13 @@
       <c r="A31" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="16" t="s">
         <v>92</v>
       </c>
       <c r="E31" s="13">
@@ -3770,13 +3773,13 @@
       <c r="A32" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="16" t="s">
         <v>90</v>
       </c>
       <c r="E32" s="13">
@@ -3787,13 +3790,13 @@
       <c r="A33" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="16" t="s">
         <v>92</v>
       </c>
       <c r="E33" s="13">
@@ -3804,13 +3807,13 @@
       <c r="A34" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="16" t="s">
         <v>92</v>
       </c>
       <c r="E34" s="13">
@@ -3821,13 +3824,13 @@
       <c r="A35" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="16" t="s">
         <v>92</v>
       </c>
       <c r="E35" s="13">
@@ -3838,13 +3841,13 @@
       <c r="A36" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="16" t="s">
         <v>98</v>
       </c>
       <c r="E36" s="13">
@@ -3855,13 +3858,13 @@
       <c r="A37" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="16" t="s">
         <v>99</v>
       </c>
       <c r="E37" s="13">
@@ -3872,13 +3875,13 @@
       <c r="A38" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D38" s="15"/>
+      <c r="D38" s="16"/>
       <c r="E38" s="13">
         <v>4.5</v>
       </c>
@@ -3887,13 +3890,13 @@
       <c r="A39" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D39" s="15"/>
+      <c r="D39" s="16"/>
       <c r="E39" s="13">
         <v>9.0</v>
       </c>
@@ -3902,13 +3905,13 @@
       <c r="A40" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D40" s="15"/>
+      <c r="D40" s="16"/>
       <c r="E40" s="13">
         <v>12.0</v>
       </c>
@@ -3917,13 +3920,13 @@
       <c r="A41" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D41" s="15"/>
+      <c r="D41" s="16"/>
       <c r="E41" s="13">
         <v>25.0</v>
       </c>
@@ -3932,13 +3935,13 @@
       <c r="A42" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="16" t="s">
         <v>107</v>
       </c>
       <c r="E42" s="13">
@@ -3949,13 +3952,13 @@
       <c r="A43" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="16" t="s">
         <v>110</v>
       </c>
       <c r="E43" s="13">
@@ -3966,13 +3969,13 @@
       <c r="A44" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E44" s="13">
@@ -3983,13 +3986,13 @@
       <c r="A45" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E45" s="13">
@@ -4000,13 +4003,13 @@
       <c r="A46" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E46" s="13">
@@ -4017,13 +4020,13 @@
       <c r="A47" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C47" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="16" t="s">
         <v>117</v>
       </c>
       <c r="E47" s="13">
@@ -4034,13 +4037,13 @@
       <c r="A48" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E48" s="13">
@@ -4051,13 +4054,13 @@
       <c r="A49" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C49" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E49" s="13">
@@ -4068,13 +4071,13 @@
       <c r="A50" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E50" s="13">
@@ -4085,13 +4088,13 @@
       <c r="A51" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E51" s="13">
@@ -4102,13 +4105,13 @@
       <c r="A52" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E52" s="13">
@@ -4119,13 +4122,13 @@
       <c r="A53" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C53" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="D53" s="15" t="s">
+      <c r="D53" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E53" s="13">
@@ -4136,13 +4139,13 @@
       <c r="A54" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C54" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E54" s="13">
@@ -4153,13 +4156,13 @@
       <c r="A55" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="C55" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="D55" s="15" t="s">
+      <c r="D55" s="16" t="s">
         <v>123</v>
       </c>
       <c r="E55" s="13">
@@ -4170,13 +4173,13 @@
       <c r="A56" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C56" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="D56" s="15" t="s">
+      <c r="D56" s="16" t="s">
         <v>125</v>
       </c>
       <c r="E56" s="13">
@@ -4187,13 +4190,13 @@
       <c r="A57" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="D57" s="15" t="s">
+      <c r="D57" s="16" t="s">
         <v>127</v>
       </c>
       <c r="E57" s="13">
@@ -4204,13 +4207,13 @@
       <c r="A58" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="16" t="s">
         <v>127</v>
       </c>
       <c r="E58" s="13">
@@ -4221,13 +4224,13 @@
       <c r="A59" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C59" s="15" t="s">
+      <c r="C59" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="D59" s="15" t="s">
+      <c r="D59" s="16" t="s">
         <v>127</v>
       </c>
       <c r="E59" s="13">
@@ -4238,13 +4241,13 @@
       <c r="A60" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="C60" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D60" s="15" t="s">
+      <c r="D60" s="16" t="s">
         <v>127</v>
       </c>
       <c r="E60" s="13">
@@ -4255,13 +4258,13 @@
       <c r="A61" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="C61" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D61" s="15" t="s">
+      <c r="D61" s="16" t="s">
         <v>127</v>
       </c>
       <c r="E61" s="13">
@@ -4272,13 +4275,13 @@
       <c r="A62" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="D62" s="16" t="s">
         <v>127</v>
       </c>
       <c r="E62" s="13">
@@ -4289,13 +4292,13 @@
       <c r="A63" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C63" s="15" t="s">
+      <c r="C63" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="D63" s="16" t="s">
         <v>127</v>
       </c>
       <c r="E63" s="13">
@@ -4306,13 +4309,13 @@
       <c r="A64" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="C64" s="15" t="s">
+      <c r="C64" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="D64" s="16" t="s">
         <v>132</v>
       </c>
       <c r="E64" s="13">
@@ -4323,13 +4326,13 @@
       <c r="A65" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B65" s="15" t="s">
+      <c r="B65" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C65" s="15" t="s">
+      <c r="C65" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="D65" s="15" t="s">
+      <c r="D65" s="16" t="s">
         <v>134</v>
       </c>
       <c r="E65" s="13">
@@ -5275,13 +5278,13 @@
       <c r="A121" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B121" s="16" t="s">
+      <c r="B121" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C121" s="16" t="s">
+      <c r="C121" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D121" s="16" t="s">
+      <c r="D121" s="17" t="s">
         <v>52</v>
       </c>
       <c r="E121" s="13">
@@ -5292,13 +5295,13 @@
       <c r="A122" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B122" s="16" t="s">
+      <c r="B122" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C122" s="16" t="s">
+      <c r="C122" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D122" s="16" t="s">
+      <c r="D122" s="17" t="s">
         <v>52</v>
       </c>
       <c r="E122" s="13">
@@ -5309,13 +5312,13 @@
       <c r="A123" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B123" s="16" t="s">
+      <c r="B123" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C123" s="16" t="s">
+      <c r="C123" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D123" s="16" t="s">
+      <c r="D123" s="17" t="s">
         <v>55</v>
       </c>
       <c r="E123" s="13">
@@ -5326,13 +5329,13 @@
       <c r="A124" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B124" s="16" t="s">
+      <c r="B124" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C124" s="16" t="s">
+      <c r="C124" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D124" s="16" t="s">
+      <c r="D124" s="17" t="s">
         <v>55</v>
       </c>
       <c r="E124" s="13">
@@ -5343,13 +5346,13 @@
       <c r="A125" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B125" s="16" t="s">
+      <c r="B125" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C125" s="16" t="s">
+      <c r="C125" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="D125" s="16" t="s">
+      <c r="D125" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E125" s="13">
@@ -5360,13 +5363,13 @@
       <c r="A126" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B126" s="16" t="s">
+      <c r="B126" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C126" s="16" t="s">
+      <c r="C126" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="D126" s="16" t="s">
+      <c r="D126" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E126" s="13">
@@ -5377,13 +5380,13 @@
       <c r="A127" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B127" s="16" t="s">
+      <c r="B127" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C127" s="16" t="s">
+      <c r="C127" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="D127" s="16" t="s">
+      <c r="D127" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E127" s="13">
@@ -5394,13 +5397,13 @@
       <c r="A128" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B128" s="16" t="s">
+      <c r="B128" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C128" s="16" t="s">
+      <c r="C128" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="D128" s="16" t="s">
+      <c r="D128" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E128" s="13">
@@ -5411,13 +5414,13 @@
       <c r="A129" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B129" s="16" t="s">
+      <c r="B129" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C129" s="16" t="s">
+      <c r="C129" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="D129" s="16" t="s">
+      <c r="D129" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E129" s="13">
@@ -5428,13 +5431,13 @@
       <c r="A130" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B130" s="16" t="s">
+      <c r="B130" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C130" s="16" t="s">
+      <c r="C130" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="D130" s="16" t="s">
+      <c r="D130" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E130" s="13">
@@ -5445,13 +5448,13 @@
       <c r="A131" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B131" s="16" t="s">
+      <c r="B131" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C131" s="16" t="s">
+      <c r="C131" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="D131" s="16" t="s">
+      <c r="D131" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E131" s="13">
@@ -5462,13 +5465,13 @@
       <c r="A132" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B132" s="16" t="s">
+      <c r="B132" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C132" s="16" t="s">
+      <c r="C132" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D132" s="16" t="s">
+      <c r="D132" s="17" t="s">
         <v>175</v>
       </c>
       <c r="E132" s="13">
@@ -5479,13 +5482,13 @@
       <c r="A133" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="16" t="s">
+      <c r="B133" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C133" s="16" t="s">
+      <c r="C133" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="D133" s="16" t="s">
+      <c r="D133" s="17" t="s">
         <v>175</v>
       </c>
       <c r="E133" s="13">
@@ -5496,13 +5499,13 @@
       <c r="A134" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B134" s="16" t="s">
+      <c r="B134" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C134" s="16" t="s">
+      <c r="C134" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D134" s="16" t="s">
+      <c r="D134" s="17" t="s">
         <v>178</v>
       </c>
       <c r="E134" s="13">
@@ -5513,13 +5516,13 @@
       <c r="A135" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B135" s="16" t="s">
+      <c r="B135" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C135" s="16" t="s">
+      <c r="C135" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="D135" s="16" t="s">
+      <c r="D135" s="17" t="s">
         <v>178</v>
       </c>
       <c r="E135" s="13">
@@ -5530,13 +5533,13 @@
       <c r="A136" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B136" s="16" t="s">
+      <c r="B136" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C136" s="16" t="s">
+      <c r="C136" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D136" s="16" t="s">
+      <c r="D136" s="17" t="s">
         <v>178</v>
       </c>
       <c r="E136" s="13">
@@ -5547,13 +5550,13 @@
       <c r="A137" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B137" s="16" t="s">
+      <c r="B137" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="C137" s="16" t="s">
+      <c r="C137" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="D137" s="16" t="s">
+      <c r="D137" s="17" t="s">
         <v>182</v>
       </c>
       <c r="E137" s="13">
@@ -5564,13 +5567,13 @@
       <c r="A138" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B138" s="16" t="s">
+      <c r="B138" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="C138" s="16" t="s">
+      <c r="C138" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="D138" s="16" t="s">
+      <c r="D138" s="17" t="s">
         <v>182</v>
       </c>
       <c r="E138" s="13">
@@ -5581,13 +5584,13 @@
       <c r="A139" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B139" s="16" t="s">
+      <c r="B139" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="C139" s="16" t="s">
+      <c r="C139" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="D139" s="16" t="s">
+      <c r="D139" s="17" t="s">
         <v>182</v>
       </c>
       <c r="E139" s="13">
@@ -5598,13 +5601,13 @@
       <c r="A140" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B140" s="16" t="s">
+      <c r="B140" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C140" s="16" t="s">
+      <c r="C140" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D140" s="16" t="s">
+      <c r="D140" s="17" t="s">
         <v>52</v>
       </c>
       <c r="E140" s="13">
@@ -5615,13 +5618,13 @@
       <c r="A141" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B141" s="16" t="s">
+      <c r="B141" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C141" s="16" t="s">
+      <c r="C141" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D141" s="16" t="s">
+      <c r="D141" s="17" t="s">
         <v>52</v>
       </c>
       <c r="E141" s="13">
@@ -5632,13 +5635,13 @@
       <c r="A142" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B142" s="16" t="s">
+      <c r="B142" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C142" s="16" t="s">
+      <c r="C142" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D142" s="16" t="s">
+      <c r="D142" s="17" t="s">
         <v>55</v>
       </c>
       <c r="E142" s="13">
@@ -5649,13 +5652,13 @@
       <c r="A143" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B143" s="16" t="s">
+      <c r="B143" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C143" s="16" t="s">
+      <c r="C143" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D143" s="16" t="s">
+      <c r="D143" s="17" t="s">
         <v>55</v>
       </c>
       <c r="E143" s="13">
@@ -5666,13 +5669,13 @@
       <c r="A144" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B144" s="16" t="s">
+      <c r="B144" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C144" s="16" t="s">
+      <c r="C144" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="D144" s="16" t="s">
+      <c r="D144" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E144" s="13">
@@ -5683,13 +5686,13 @@
       <c r="A145" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B145" s="16" t="s">
+      <c r="B145" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C145" s="16" t="s">
+      <c r="C145" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="D145" s="16" t="s">
+      <c r="D145" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E145" s="13">
@@ -5700,13 +5703,13 @@
       <c r="A146" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B146" s="16" t="s">
+      <c r="B146" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C146" s="16" t="s">
+      <c r="C146" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="D146" s="16" t="s">
+      <c r="D146" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E146" s="13">
@@ -5717,13 +5720,13 @@
       <c r="A147" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B147" s="16" t="s">
+      <c r="B147" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C147" s="16" t="s">
+      <c r="C147" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="D147" s="16" t="s">
+      <c r="D147" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E147" s="13">
@@ -5734,13 +5737,13 @@
       <c r="A148" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B148" s="16" t="s">
+      <c r="B148" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C148" s="16" t="s">
+      <c r="C148" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D148" s="16" t="s">
+      <c r="D148" s="17" t="s">
         <v>175</v>
       </c>
       <c r="E148" s="13">
@@ -5751,13 +5754,13 @@
       <c r="A149" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B149" s="16" t="s">
+      <c r="B149" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C149" s="16" t="s">
+      <c r="C149" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="D149" s="16" t="s">
+      <c r="D149" s="17" t="s">
         <v>175</v>
       </c>
       <c r="E149" s="13">
@@ -5768,13 +5771,13 @@
       <c r="A150" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B150" s="16" t="s">
+      <c r="B150" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C150" s="16" t="s">
+      <c r="C150" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D150" s="16" t="s">
+      <c r="D150" s="17" t="s">
         <v>178</v>
       </c>
       <c r="E150" s="13">
@@ -5785,13 +5788,13 @@
       <c r="A151" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B151" s="16" t="s">
+      <c r="B151" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C151" s="16" t="s">
+      <c r="C151" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="D151" s="16" t="s">
+      <c r="D151" s="17" t="s">
         <v>178</v>
       </c>
       <c r="E151" s="13">
@@ -5802,13 +5805,13 @@
       <c r="A152" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B152" s="16" t="s">
+      <c r="B152" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C152" s="16" t="s">
+      <c r="C152" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="D152" s="16" t="s">
+      <c r="D152" s="17" t="s">
         <v>178</v>
       </c>
       <c r="E152" s="13">
@@ -5819,13 +5822,13 @@
       <c r="A153" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B153" s="16" t="s">
+      <c r="B153" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C153" s="16" t="s">
+      <c r="C153" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="D153" s="16" t="s">
+      <c r="D153" s="17" t="s">
         <v>178</v>
       </c>
       <c r="E153" s="13">
@@ -5836,13 +5839,13 @@
       <c r="A154" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B154" s="16" t="s">
+      <c r="B154" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="C154" s="16" t="s">
+      <c r="C154" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="D154" s="16" t="s">
+      <c r="D154" s="17" t="s">
         <v>182</v>
       </c>
       <c r="E154" s="13">
@@ -5853,13 +5856,13 @@
       <c r="A155" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B155" s="16" t="s">
+      <c r="B155" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="C155" s="16" t="s">
+      <c r="C155" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="D155" s="16" t="s">
+      <c r="D155" s="17" t="s">
         <v>182</v>
       </c>
       <c r="E155" s="13">
@@ -5870,13 +5873,13 @@
       <c r="A156" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B156" s="16" t="s">
+      <c r="B156" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="C156" s="16" t="s">
+      <c r="C156" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="D156" s="16" t="s">
+      <c r="D156" s="17" t="s">
         <v>182</v>
       </c>
       <c r="E156" s="13">
@@ -5887,13 +5890,13 @@
       <c r="A157" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B157" s="16" t="s">
+      <c r="B157" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C157" s="16" t="s">
+      <c r="C157" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D157" s="16" t="s">
+      <c r="D157" s="17" t="s">
         <v>52</v>
       </c>
       <c r="E157" s="13">
@@ -5904,13 +5907,13 @@
       <c r="A158" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B158" s="16" t="s">
+      <c r="B158" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C158" s="16" t="s">
+      <c r="C158" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D158" s="16" t="s">
+      <c r="D158" s="17" t="s">
         <v>52</v>
       </c>
       <c r="E158" s="13">
@@ -5921,13 +5924,13 @@
       <c r="A159" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B159" s="16" t="s">
+      <c r="B159" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C159" s="16" t="s">
+      <c r="C159" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D159" s="16" t="s">
+      <c r="D159" s="17" t="s">
         <v>55</v>
       </c>
       <c r="E159" s="13">
@@ -5938,13 +5941,13 @@
       <c r="A160" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B160" s="16" t="s">
+      <c r="B160" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C160" s="16" t="s">
+      <c r="C160" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D160" s="16" t="s">
+      <c r="D160" s="17" t="s">
         <v>55</v>
       </c>
       <c r="E160" s="13">
@@ -5955,13 +5958,13 @@
       <c r="A161" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B161" s="16" t="s">
+      <c r="B161" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C161" s="16" t="s">
+      <c r="C161" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="D161" s="16" t="s">
+      <c r="D161" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E161" s="13">
@@ -5972,13 +5975,13 @@
       <c r="A162" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B162" s="16" t="s">
+      <c r="B162" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C162" s="16" t="s">
+      <c r="C162" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="D162" s="16" t="s">
+      <c r="D162" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E162" s="13">
@@ -5989,13 +5992,13 @@
       <c r="A163" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B163" s="16" t="s">
+      <c r="B163" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C163" s="16" t="s">
+      <c r="C163" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="D163" s="16" t="s">
+      <c r="D163" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E163" s="13">
@@ -6006,13 +6009,13 @@
       <c r="A164" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B164" s="16" t="s">
+      <c r="B164" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C164" s="16" t="s">
+      <c r="C164" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D164" s="16" t="s">
+      <c r="D164" s="17" t="s">
         <v>175</v>
       </c>
       <c r="E164" s="13">
@@ -6023,13 +6026,13 @@
       <c r="A165" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B165" s="16" t="s">
+      <c r="B165" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C165" s="16" t="s">
+      <c r="C165" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="D165" s="16" t="s">
+      <c r="D165" s="17" t="s">
         <v>175</v>
       </c>
       <c r="E165" s="13">
@@ -6040,13 +6043,13 @@
       <c r="A166" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B166" s="16" t="s">
+      <c r="B166" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C166" s="16" t="s">
+      <c r="C166" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="D166" s="16" t="s">
+      <c r="D166" s="17" t="s">
         <v>175</v>
       </c>
       <c r="E166" s="13">
@@ -6057,13 +6060,13 @@
       <c r="A167" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B167" s="16" t="s">
+      <c r="B167" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C167" s="16" t="s">
+      <c r="C167" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="D167" s="16" t="s">
+      <c r="D167" s="17" t="s">
         <v>175</v>
       </c>
       <c r="E167" s="13">
@@ -6074,13 +6077,13 @@
       <c r="A168" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B168" s="16" t="s">
+      <c r="B168" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C168" s="16" t="s">
+      <c r="C168" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D168" s="16" t="s">
+      <c r="D168" s="17" t="s">
         <v>178</v>
       </c>
       <c r="E168" s="13">
@@ -6091,13 +6094,13 @@
       <c r="A169" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B169" s="16" t="s">
+      <c r="B169" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C169" s="16" t="s">
+      <c r="C169" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="D169" s="16" t="s">
+      <c r="D169" s="17" t="s">
         <v>178</v>
       </c>
       <c r="E169" s="13">
@@ -6108,13 +6111,13 @@
       <c r="A170" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B170" s="16" t="s">
+      <c r="B170" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C170" s="16" t="s">
+      <c r="C170" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="D170" s="16" t="s">
+      <c r="D170" s="17" t="s">
         <v>178</v>
       </c>
       <c r="E170" s="13">
@@ -6125,13 +6128,13 @@
       <c r="A171" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B171" s="16" t="s">
+      <c r="B171" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C171" s="16" t="s">
+      <c r="C171" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="D171" s="16" t="s">
+      <c r="D171" s="17" t="s">
         <v>178</v>
       </c>
       <c r="E171" s="13">
@@ -6142,13 +6145,13 @@
       <c r="A172" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B172" s="16" t="s">
+      <c r="B172" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="C172" s="16" t="s">
+      <c r="C172" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="D172" s="16" t="s">
+      <c r="D172" s="17" t="s">
         <v>182</v>
       </c>
       <c r="E172" s="13">
@@ -6312,13 +6315,13 @@
       <c r="A182" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B182" s="17" t="s">
+      <c r="B182" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="C182" s="17" t="s">
+      <c r="C182" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="D182" s="18" t="s">
+      <c r="D182" s="19" t="s">
         <v>182</v>
       </c>
       <c r="E182" s="13"/>
@@ -6327,13 +6330,13 @@
       <c r="A183" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B183" s="17" t="s">
+      <c r="B183" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="C183" s="17" t="s">
+      <c r="C183" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="D183" s="18" t="s">
+      <c r="D183" s="19" t="s">
         <v>182</v>
       </c>
       <c r="E183" s="13"/>
@@ -6342,13 +6345,13 @@
       <c r="A184" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B184" s="17" t="s">
+      <c r="B184" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="C184" s="17" t="s">
+      <c r="C184" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="D184" s="18" t="s">
+      <c r="D184" s="19" t="s">
         <v>182</v>
       </c>
       <c r="E184" s="13"/>

</xml_diff>